<commit_message>
Enchances BarPrices.xls with the test case LTD50
</commit_message>
<xml_diff>
--- a/SsbHedger/Documentation/BarPrices.xlsx
+++ b/SsbHedger/Documentation/BarPrices.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r\Rollover\SsbHedger\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C2B806-35FA-4692-B1E5-204EAC98D781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958CF406-CF00-4FF7-A77C-2280B2DDDF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LTD 00" sheetId="1" r:id="rId1"/>
+    <sheet name="LTD 50" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Heigth 150</t>
   </si>
@@ -130,6 +131,70 @@
   </si>
   <si>
     <t>Step and First</t>
+  </si>
+  <si>
+    <t>LTD 50</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Height 150: -&gt; Net height 80% -&gt; 120; 30p/lbl-&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 lbls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; Range=15; NetRange=15*5%=0,75;MinNet = 175 +0,75= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>175,75</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; MaxNet=190-0,75=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>189,25</t>
+    </r>
+  </si>
+  <si>
+    <t>LabelStep = (189,25 - 175,75)/4 =</t>
   </si>
 </sst>
 </file>
@@ -197,98 +262,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>816429</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>65315</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>119743</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Speech Bubble: Oval 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A3102F1-9DEF-E9CB-DD0B-09B1AE163814}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5040086" y="1905000"/>
-          <a:ext cx="3929743" cy="620486"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeEllipseCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -56644"/>
-            <a:gd name="adj2" fmla="val 60746"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="2000">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Uneven</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="de-DE" sz="2000">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>steps!</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100"/>
-            <a:t>!</a:t>
-          </a:r>
-          <a:endParaRPr lang="LID4096" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -556,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,12 +651,7 @@
         <v>185.13</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <v>185.5</v>
-      </c>
-      <c r="H9">
-        <v>185.25</v>
-      </c>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -757,14 +725,10 @@
         <v>178.38</v>
       </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <v>178.5</v>
-      </c>
-      <c r="H16" s="2">
-        <v>178.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>177</v>
       </c>
@@ -774,7 +738,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>176</v>
       </c>
@@ -784,7 +748,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>175</v>
       </c>
@@ -793,7 +757,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>174</v>
       </c>
@@ -803,7 +767,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>173</v>
       </c>
@@ -813,7 +777,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>172</v>
       </c>
@@ -823,11 +787,9 @@
       <c r="F22" s="2">
         <v>172</v>
       </c>
-      <c r="G22" s="2">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>171</v>
       </c>
@@ -837,11 +799,8 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23">
-        <v>171.75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>170</v>
       </c>
@@ -851,7 +810,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>169</v>
       </c>
@@ -861,7 +820,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>168</v>
       </c>
@@ -871,7 +830,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>167</v>
       </c>
@@ -881,7 +840,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>166</v>
       </c>
@@ -891,7 +850,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>165</v>
       </c>
@@ -901,14 +860,9 @@
       <c r="F29" s="2">
         <v>165</v>
       </c>
-      <c r="G29" s="2">
-        <v>165</v>
-      </c>
-      <c r="H29">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>164</v>
       </c>
@@ -919,7 +873,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>163</v>
       </c>
@@ -929,7 +883,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>162</v>
       </c>
@@ -1004,6 +958,388 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6547C17-3FEC-4EC1-99CF-8D38DDBE3FB9}">
+  <dimension ref="A1:L41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1">
+        <v>25</v>
+      </c>
+      <c r="H1">
+        <v>20</v>
+      </c>
+      <c r="I1">
+        <v>10</v>
+      </c>
+      <c r="J1">
+        <v>5</v>
+      </c>
+      <c r="K1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>190</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>189.5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>189.25</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>189</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>188.5</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>188</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>187.5</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>187.57999999999998</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>187</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>186.5</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>186</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>185.5</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>185</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>184.5</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="F15" s="2">
+        <v>184.5</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>184</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2">
+        <v>184.2</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>183.5</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>183</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>182.5</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>182</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>181.5</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>181</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="F22" s="2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>180.5</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2">
+        <v>180.82</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>180</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>179.5</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>179</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>178.5</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>178</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>177.5</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="F29" s="2">
+        <v>177.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>177</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2">
+        <v>177.44</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>176.5</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>176</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>175.5</v>
+      </c>
+      <c r="C33" s="2">
+        <v>175.75</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>175</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="4">
+        <v>3.38</v>
+      </c>
+      <c r="I38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1.69</v>
+      </c>
+      <c r="L38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Extends BarPrices.xls with new test data
</commit_message>
<xml_diff>
--- a/SsbHedger/Documentation/BarPrices.xlsx
+++ b/SsbHedger/Documentation/BarPrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r\Rollover\SsbHedger\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B28AABB-6440-4CD4-B829-69A74F4BEC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFB38D4-6A91-410B-884B-83C6EE766A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTD 00" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="LTD 05" sheetId="6" r:id="rId6"/>
     <sheet name="LTD 02" sheetId="7" r:id="rId7"/>
     <sheet name="SampleFromCode" sheetId="8" r:id="rId8"/>
+    <sheet name="ReturnListOfPriceAndMargin" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
   <si>
     <t>Heigth 150</t>
   </si>
@@ -595,6 +596,54 @@
   <si>
     <t>step/2</t>
   </si>
+  <si>
+    <t>AxisHeight</t>
+  </si>
+  <si>
+    <t>MinHeightLabel</t>
+  </si>
+  <si>
+    <t>ChartBuffer</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>AxisNetHeight</t>
+  </si>
+  <si>
+    <t>NumberOfLabels</t>
+  </si>
+  <si>
+    <t>PointsPerLabelStep</t>
+  </si>
+  <si>
+    <t>LabelSteps</t>
+  </si>
+  <si>
+    <t>PricePerLabelStep</t>
+  </si>
+  <si>
+    <t>RangePrice</t>
+  </si>
+  <si>
+    <t>MaxRangePrice</t>
+  </si>
+  <si>
+    <t>MinRangePrice</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
 </sst>
 </file>
 
@@ -606,7 +655,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,6 +671,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -631,7 +695,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -639,11 +703,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -654,9 +777,49 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3536,9 +3699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E00779-A7A8-475A-ACFE-7A59F9649B0E}">
   <dimension ref="A1:M136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4316,4 +4479,275 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4108A046-A224-4C38-B22F-2182BCD6D4B7}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <f>$B$4*(1-$E$3*2)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <f>$B$4*$E$3</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <f>B7/E2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <f>B9-1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <f>B7/B12</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <f>$B$2-$B$3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <f>B16/B12</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="20">
+        <v>10</v>
+      </c>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="23">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13">
+        <v>36</v>
+      </c>
+      <c r="C23" s="23"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="23">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13">
+        <v>36</v>
+      </c>
+      <c r="C25" s="23"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="23">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13">
+        <v>36</v>
+      </c>
+      <c r="C27" s="23"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="13">
+        <v>36</v>
+      </c>
+      <c r="C29" s="23"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="13">
+        <v>36</v>
+      </c>
+      <c r="C31" s="23"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="16">
+        <v>10</v>
+      </c>
+      <c r="C33" s="23"/>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="24"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="17"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="26">
+        <f>SUM(B21:B34)</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C22:C23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>